<commit_message>
Ramal agua retirado do escopo
</commit_message>
<xml_diff>
--- a/sheets/estoque.XLSX
+++ b/sheets/estoque.XLSX
@@ -3313,13 +3313,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>4156.000</v>
+        <v>4155.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>42818.30</v>
+        <v>42807.99</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -4197,13 +4197,13 @@
         <v>156</v>
       </c>
       <c r="F78" s="2">
-        <v>900.000</v>
+        <v>898.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>4678.37</v>
+        <v>4667.97</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -4743,13 +4743,13 @@
         <v>198</v>
       </c>
       <c r="F99" s="2">
-        <v>2370.000</v>
+        <v>2368.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>62180.03</v>
+        <v>62127.55</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -5133,13 +5133,13 @@
         <v>228</v>
       </c>
       <c r="F114" s="2">
-        <v>330.000</v>
+        <v>328.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>189813.78</v>
+        <v>188663.39</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -5159,13 +5159,13 @@
         <v>230</v>
       </c>
       <c r="F115" s="2">
-        <v>2550.000</v>
+        <v>2548.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>217935.75</v>
+        <v>217764.82</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -5185,13 +5185,13 @@
         <v>232</v>
       </c>
       <c r="F116" s="2">
-        <v>3501.000</v>
+        <v>3478.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>482244.98</v>
+        <v>479076.90</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -5497,13 +5497,13 @@
         <v>256</v>
       </c>
       <c r="F128" s="2">
-        <v>938.000</v>
+        <v>937.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>35282.87</v>
+        <v>35245.25</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5679,13 +5679,13 @@
         <v>270</v>
       </c>
       <c r="F135" s="2">
-        <v>3817.000</v>
+        <v>3785.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>14758.02</v>
+        <v>14634.28</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -7369,13 +7369,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>986.000</v>
+        <v>985.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>188660.10</v>
+        <v>188468.76</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -10125,13 +10125,13 @@
         <v>614</v>
       </c>
       <c r="F306" s="2">
-        <v>7138.530</v>
+        <v>7135.530</v>
       </c>
       <c r="G306" t="s">
         <v>562</v>
       </c>
       <c r="H306" s="3">
-        <v>72913.34</v>
+        <v>72882.70</v>
       </c>
     </row>
     <row r="307" spans="1:8">

</xml_diff>

<commit_message>
Adding sleep in main.rs
</commit_message>
<xml_diff>
--- a/sheets/estoque.XLSX
+++ b/sheets/estoque.XLSX
@@ -4771,13 +4771,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>69.000</v>
+        <v>67.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>7032.31</v>
+        <v>6828.47</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -6305,13 +6305,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>3432.000</v>
+        <v>1332.000</v>
       </c>
       <c r="G175" t="s">
         <v>351</v>
       </c>
       <c r="H175" s="3">
-        <v>5131.65</v>
+        <v>1991.65</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6487,13 +6487,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>98.000</v>
+        <v>97.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>45447.92</v>
+        <v>44984.17</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -7969,13 +7969,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>1503.980</v>
+        <v>1488.860</v>
       </c>
       <c r="G239" t="s">
         <v>440</v>
       </c>
       <c r="H239" s="3">
-        <v>47249.72</v>
+        <v>46774.71</v>
       </c>
     </row>
     <row r="240" spans="1:8">

</xml_diff>

<commit_message>
#fix: services without hidro serial number and put lacre step-by-step
</commit_message>
<xml_diff>
--- a/sheets/estoque.XLSX
+++ b/sheets/estoque.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="541">
   <si>
     <t>4600041302</t>
   </si>
@@ -593,12 +593,6 @@
   </si>
   <si>
     <t>HIDRANTE SUBT C/BASE FLANG DN 75 SIMPLES</t>
-  </si>
-  <si>
-    <t>50000108</t>
-  </si>
-  <si>
-    <t>HIDRO UNIJATO DN20 QN0,75 M³/H - PRE-EQ</t>
   </si>
   <si>
     <t>50000530</t>
@@ -1746,7 +1740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H266"/>
+  <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,28 +1760,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>541</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4277,13 +4271,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>1.000</v>
+        <v>2369.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>85.47</v>
+        <v>326318.48</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4303,13 +4297,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>2369.000</v>
+        <v>1.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>326318.48</v>
+        <v>2980.59</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4335,7 +4329,7 @@
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>2980.59</v>
+        <v>4463.84</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4355,13 +4349,13 @@
         <v>201</v>
       </c>
       <c r="F100" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G100" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>4463.84</v>
+        <v>1598.31</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4381,13 +4375,13 @@
         <v>203</v>
       </c>
       <c r="F101" s="2">
-        <v>3.000</v>
+        <v>20.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>1598.31</v>
+        <v>24666.05</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4407,13 +4401,13 @@
         <v>205</v>
       </c>
       <c r="F102" s="2">
-        <v>20.000</v>
+        <v>6.000</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>24666.05</v>
+        <v>10134.33</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4433,13 +4427,13 @@
         <v>207</v>
       </c>
       <c r="F103" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G103" t="s">
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>10134.33</v>
+        <v>751.71</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4459,13 +4453,13 @@
         <v>209</v>
       </c>
       <c r="F104" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>751.71</v>
+        <v>279.59</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4485,13 +4479,13 @@
         <v>211</v>
       </c>
       <c r="F105" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G105" t="s">
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>279.59</v>
+        <v>740.97</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -4517,7 +4511,7 @@
         <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>740.97</v>
+        <v>902.80</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -4543,7 +4537,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>902.80</v>
+        <v>1166.57</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4563,13 +4557,13 @@
         <v>217</v>
       </c>
       <c r="F108" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G108" t="s">
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>1166.57</v>
+        <v>2825.06</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4589,13 +4583,13 @@
         <v>219</v>
       </c>
       <c r="F109" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>2825.06</v>
+        <v>91.20</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4615,13 +4609,13 @@
         <v>221</v>
       </c>
       <c r="F110" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G110" t="s">
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>91.20</v>
+        <v>719.47</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4641,13 +4635,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>2.000</v>
+        <v>514.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>719.47</v>
+        <v>19074.89</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4667,13 +4661,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>514.000</v>
+        <v>352.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>19074.89</v>
+        <v>23009.79</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4693,13 +4687,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>352.000</v>
+        <v>892.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>23009.79</v>
+        <v>29388.73</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4719,13 +4713,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>892.000</v>
+        <v>176.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>29388.73</v>
+        <v>9043.46</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4745,13 +4739,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>176.000</v>
+        <v>67.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>9043.46</v>
+        <v>6828.47</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4771,13 +4765,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>67.000</v>
+        <v>45.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>6828.47</v>
+        <v>1519.40</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4797,13 +4791,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>45.000</v>
+        <v>9.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>1519.40</v>
+        <v>1675.75</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4823,13 +4817,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>9.000</v>
+        <v>4788.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>1675.75</v>
+        <v>18512.01</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4849,13 +4843,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>4789.000</v>
+        <v>2.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>18515.88</v>
+        <v>2463.85</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4881,7 +4875,7 @@
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>2463.85</v>
+        <v>4533.88</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4901,13 +4895,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>4533.88</v>
+        <v>6385.34</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4927,13 +4921,13 @@
         <v>245</v>
       </c>
       <c r="F122" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>6385.34</v>
+        <v>12368.67</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4953,13 +4947,13 @@
         <v>247</v>
       </c>
       <c r="F123" s="2">
-        <v>6.000</v>
+        <v>3.000</v>
       </c>
       <c r="G123" t="s">
         <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>12368.67</v>
+        <v>3260.53</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4979,13 +4973,13 @@
         <v>249</v>
       </c>
       <c r="F124" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>3260.53</v>
+        <v>3527.49</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -5005,13 +4999,13 @@
         <v>251</v>
       </c>
       <c r="F125" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G125" t="s">
         <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>3527.49</v>
+        <v>6294.26</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5031,13 +5025,13 @@
         <v>253</v>
       </c>
       <c r="F126" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G126" t="s">
         <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>6294.26</v>
+        <v>4585.00</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5063,7 +5057,7 @@
         <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>4585.00</v>
+        <v>7112.72</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -5083,13 +5077,13 @@
         <v>257</v>
       </c>
       <c r="F128" s="2">
-        <v>1.000</v>
+        <v>71.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>7112.72</v>
+        <v>102407.91</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5109,13 +5103,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>71.000</v>
+        <v>562.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>102407.91</v>
+        <v>3181.36</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5135,13 +5129,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>562.000</v>
+        <v>261.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>3181.36</v>
+        <v>2053.95</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5161,13 +5155,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>261.000</v>
+        <v>92.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>2053.95</v>
+        <v>1442.37</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5187,13 +5181,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>92.000</v>
+        <v>113.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>1442.37</v>
+        <v>1540.59</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5213,13 +5207,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>113.000</v>
+        <v>44.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1540.59</v>
+        <v>1343.00</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5239,13 +5233,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>44.000</v>
+        <v>28.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>1343.00</v>
+        <v>3185.96</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5265,13 +5259,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>28.000</v>
+        <v>1.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>3185.96</v>
+        <v>194.13</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5291,13 +5285,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>194.13</v>
+        <v>159.15</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5323,7 +5317,7 @@
         <v>5</v>
       </c>
       <c r="H137" s="3">
-        <v>159.15</v>
+        <v>499.74</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5343,13 +5337,13 @@
         <v>277</v>
       </c>
       <c r="F138" s="2">
-        <v>2.000</v>
+        <v>43.000</v>
       </c>
       <c r="G138" t="s">
         <v>5</v>
       </c>
       <c r="H138" s="3">
-        <v>499.74</v>
+        <v>3120.30</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5369,13 +5363,13 @@
         <v>279</v>
       </c>
       <c r="F139" s="2">
-        <v>43.000</v>
+        <v>15.000</v>
       </c>
       <c r="G139" t="s">
         <v>5</v>
       </c>
       <c r="H139" s="3">
-        <v>3120.30</v>
+        <v>2283.44</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5395,13 +5389,13 @@
         <v>281</v>
       </c>
       <c r="F140" s="2">
-        <v>15.000</v>
+        <v>12.000</v>
       </c>
       <c r="G140" t="s">
         <v>5</v>
       </c>
       <c r="H140" s="3">
-        <v>2283.44</v>
+        <v>5668.76</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5421,13 +5415,13 @@
         <v>283</v>
       </c>
       <c r="F141" s="2">
-        <v>12.000</v>
+        <v>10.000</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
       </c>
       <c r="H141" s="3">
-        <v>5668.76</v>
+        <v>6951.09</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5447,13 +5441,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="2">
-        <v>10.000</v>
+        <v>4.000</v>
       </c>
       <c r="G142" t="s">
         <v>5</v>
       </c>
       <c r="H142" s="3">
-        <v>6951.09</v>
+        <v>3749.58</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5473,13 +5467,13 @@
         <v>287</v>
       </c>
       <c r="F143" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="G143" t="s">
         <v>5</v>
       </c>
       <c r="H143" s="3">
-        <v>3749.58</v>
+        <v>5800.85</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5499,13 +5493,13 @@
         <v>289</v>
       </c>
       <c r="F144" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
       </c>
       <c r="H144" s="3">
-        <v>5800.85</v>
+        <v>5120.09</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5525,13 +5519,13 @@
         <v>291</v>
       </c>
       <c r="F145" s="2">
-        <v>3.000</v>
+        <v>5.000</v>
       </c>
       <c r="G145" t="s">
         <v>5</v>
       </c>
       <c r="H145" s="3">
-        <v>5120.09</v>
+        <v>1690.54</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5551,13 +5545,13 @@
         <v>293</v>
       </c>
       <c r="F146" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
       </c>
       <c r="H146" s="3">
-        <v>1690.54</v>
+        <v>1642.41</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5577,13 +5571,13 @@
         <v>295</v>
       </c>
       <c r="F147" s="2">
-        <v>6.000</v>
+        <v>20.000</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
       </c>
       <c r="H147" s="3">
-        <v>1642.41</v>
+        <v>5922.04</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5603,13 +5597,13 @@
         <v>297</v>
       </c>
       <c r="F148" s="2">
-        <v>20.000</v>
+        <v>3.000</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
       </c>
       <c r="H148" s="3">
-        <v>5922.04</v>
+        <v>162.71</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5629,13 +5623,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>3.000</v>
+        <v>4.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>162.71</v>
+        <v>419.08</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5655,13 +5649,13 @@
         <v>301</v>
       </c>
       <c r="F150" s="2">
-        <v>4.000</v>
+        <v>30.000</v>
       </c>
       <c r="G150" t="s">
         <v>5</v>
       </c>
       <c r="H150" s="3">
-        <v>419.08</v>
+        <v>179.61</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5681,13 +5675,13 @@
         <v>303</v>
       </c>
       <c r="F151" s="2">
-        <v>30.000</v>
+        <v>6.000</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
       </c>
       <c r="H151" s="3">
-        <v>179.61</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5707,13 +5701,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>98.34</v>
+        <v>374.16</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5733,13 +5727,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>10.000</v>
+        <v>575.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>374.16</v>
+        <v>2545.17</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5759,13 +5753,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>575.000</v>
+        <v>16.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>2545.17</v>
+        <v>1204.47</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5785,13 +5779,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>16.000</v>
+        <v>2.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>1204.47</v>
+        <v>270.71</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5811,13 +5805,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>2.000</v>
+        <v>25.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>270.71</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5837,13 +5831,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>25.000</v>
+        <v>10.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>116.25</v>
+        <v>1194.56</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5863,13 +5857,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>10.000</v>
+        <v>30.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>1194.56</v>
+        <v>3064.98</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5889,13 +5883,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>30.000</v>
+        <v>54.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>3064.98</v>
+        <v>7209.49</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5915,13 +5909,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>54.000</v>
+        <v>1.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>7209.49</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5938,16 +5932,16 @@
         <v>322</v>
       </c>
       <c r="E161" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F161" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>40.71</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5961,19 +5955,19 @@
         <v>2</v>
       </c>
       <c r="D162" t="s">
+        <v>323</v>
+      </c>
+      <c r="E162" t="s">
         <v>324</v>
       </c>
-      <c r="E162" t="s">
-        <v>323</v>
-      </c>
       <c r="F162" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>317.81</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5999,7 +5993,7 @@
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>483.20</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6019,13 +6013,13 @@
         <v>328</v>
       </c>
       <c r="F164" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G164" t="s">
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>45.92</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6051,7 +6045,7 @@
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>303.12</v>
+        <v>266.42</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6071,13 +6065,13 @@
         <v>332</v>
       </c>
       <c r="F166" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G166" t="s">
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>266.42</v>
+        <v>1141.60</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6097,13 +6091,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>8.000</v>
+        <v>3.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>1141.60</v>
+        <v>1028.70</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6123,13 +6117,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>3.000</v>
+        <v>9.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>1028.70</v>
+        <v>543.81</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6149,13 +6143,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>9.000</v>
+        <v>2.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>543.81</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6175,13 +6169,13 @@
         <v>340</v>
       </c>
       <c r="F170" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>412.45</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6201,13 +6195,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>24.27</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6227,13 +6221,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>9.000</v>
+        <v>15.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>214.33</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6253,13 +6247,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>15.000</v>
+        <v>1990.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>3032.79</v>
+        <v>37262.79</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6279,13 +6273,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>1990.000</v>
+        <v>1332.000</v>
       </c>
       <c r="G174" t="s">
-        <v>5</v>
+        <v>349</v>
       </c>
       <c r="H174" s="3">
-        <v>37262.79</v>
+        <v>1991.65</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6299,19 +6293,19 @@
         <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E175" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F175" s="2">
-        <v>1332.000</v>
+        <v>103.000</v>
       </c>
       <c r="G175" t="s">
-        <v>351</v>
+        <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>1991.65</v>
+        <v>3671.30</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6331,13 +6325,13 @@
         <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>103.000</v>
+        <v>13.000</v>
       </c>
       <c r="G176" t="s">
         <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>3671.30</v>
+        <v>2487.40</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6357,13 +6351,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>13.000</v>
+        <v>658.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>2487.40</v>
+        <v>114898.06</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6383,13 +6377,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>658.000</v>
+        <v>7.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>114898.06</v>
+        <v>1219.43</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6409,13 +6403,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>7.000</v>
+        <v>11.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>1219.43</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6435,13 +6429,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>11.000</v>
+        <v>22.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>145.79</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6461,13 +6455,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>22.000</v>
+        <v>97.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>10363.87</v>
+        <v>44984.17</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6487,13 +6481,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>97.000</v>
+        <v>26.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>44984.17</v>
+        <v>1587.82</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6513,13 +6507,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>26.000</v>
+        <v>88.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>1587.82</v>
+        <v>12845.15</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6539,13 +6533,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>88.000</v>
+        <v>1.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>12845.15</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6571,7 +6565,7 @@
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>1218.18</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6591,13 +6585,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>1.000</v>
+        <v>184.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1720.00</v>
+        <v>6147.25</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6617,13 +6611,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>184.000</v>
+        <v>28.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>6147.25</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6643,13 +6637,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>28.000</v>
+        <v>459.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>1119.31</v>
+        <v>7175.19</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6669,13 +6663,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>459.000</v>
+        <v>59.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>7175.19</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6695,13 +6689,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>59.000</v>
+        <v>502.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>1003.06</v>
+        <v>10170.52</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6721,13 +6715,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>502.000</v>
+        <v>44.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>10170.52</v>
+        <v>1021.95</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6747,13 +6741,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>44.000</v>
+        <v>96.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>1021.95</v>
+        <v>6840.48</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6773,13 +6767,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>96.000</v>
+        <v>22.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>6840.48</v>
+        <v>2460.83</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6799,13 +6793,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>22.000</v>
+        <v>1.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>2460.83</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6825,13 +6819,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>189.22</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6851,13 +6845,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>19.000</v>
+        <v>299.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>1201.67</v>
+        <v>20704.25</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6877,13 +6871,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>299.000</v>
+        <v>2.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>20704.25</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6903,13 +6897,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>651.09</v>
+        <v>562.67</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6935,7 +6929,7 @@
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>562.67</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6955,13 +6949,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>1125.55</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6981,13 +6975,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>718.30</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7013,7 +7007,7 @@
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>266.26</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7033,13 +7027,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>257.36</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7059,13 +7053,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>961.64</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7085,13 +7079,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>726.22</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7111,13 +7105,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>662.53</v>
+        <v>493.11</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7137,13 +7131,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>493.11</v>
+        <v>885.89</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7163,13 +7157,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>7.000</v>
+        <v>41.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>885.89</v>
+        <v>5647.65</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7189,13 +7183,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>41.000</v>
+        <v>1.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>5647.65</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7221,7 +7215,7 @@
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>4700.00</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7241,13 +7235,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>1.000</v>
+        <v>40.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>8560.17</v>
+        <v>506.58</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7267,13 +7261,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>40.000</v>
+        <v>1.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>506.58</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7293,13 +7287,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>1.000</v>
+        <v>11.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>23.34</v>
+        <v>418.00</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7319,13 +7313,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>11.000</v>
+        <v>24.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>418.00</v>
+        <v>1584.75</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7345,13 +7339,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>24.000</v>
+        <v>1.000</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
       </c>
       <c r="H215" s="3">
-        <v>1584.75</v>
+        <v>29.64</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7377,7 +7371,7 @@
         <v>5</v>
       </c>
       <c r="H216" s="3">
-        <v>29.64</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7397,13 +7391,13 @@
         <v>435</v>
       </c>
       <c r="F217" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G217" t="s">
         <v>5</v>
       </c>
       <c r="H217" s="3">
-        <v>685.11</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7423,13 +7417,13 @@
         <v>437</v>
       </c>
       <c r="F218" s="2">
-        <v>2.000</v>
+        <v>4.800</v>
       </c>
       <c r="G218" t="s">
-        <v>5</v>
+        <v>438</v>
       </c>
       <c r="H218" s="3">
-        <v>8149.76</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7443,19 +7437,19 @@
         <v>2</v>
       </c>
       <c r="D219" t="s">
+        <v>439</v>
+      </c>
+      <c r="E219" t="s">
+        <v>440</v>
+      </c>
+      <c r="F219" s="2">
+        <v>16.000</v>
+      </c>
+      <c r="G219" t="s">
         <v>438</v>
       </c>
-      <c r="E219" t="s">
-        <v>439</v>
-      </c>
-      <c r="F219" s="2">
-        <v>4.800</v>
-      </c>
-      <c r="G219" t="s">
-        <v>440</v>
-      </c>
       <c r="H219" s="3">
-        <v>1822.34</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7475,13 +7469,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>16.000</v>
+        <v>17.000</v>
       </c>
       <c r="G220" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H220" s="3">
-        <v>7011.29</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7501,13 +7495,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>17.000</v>
+        <v>184.000</v>
       </c>
       <c r="G221" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H221" s="3">
-        <v>2938.94</v>
+        <v>39969.93</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7527,13 +7521,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>184.000</v>
+        <v>1.090</v>
       </c>
       <c r="G222" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H222" s="3">
-        <v>39969.93</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7553,13 +7547,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>1.090</v>
+        <v>20.300</v>
       </c>
       <c r="G223" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H223" s="3">
-        <v>250.66</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7579,13 +7573,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>20.300</v>
+        <v>13.000</v>
       </c>
       <c r="G224" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H224" s="3">
-        <v>6816.84</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7605,13 +7599,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>13.000</v>
+        <v>22.000</v>
       </c>
       <c r="G225" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H225" s="3">
-        <v>3437.72</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7631,13 +7625,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>22.000</v>
+        <v>345.400</v>
       </c>
       <c r="G226" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H226" s="3">
-        <v>2084.93</v>
+        <v>3460.95</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7657,13 +7651,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>345.400</v>
+        <v>99.000</v>
       </c>
       <c r="G227" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H227" s="3">
-        <v>3460.95</v>
+        <v>2142.16</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7683,13 +7677,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>99.000</v>
+        <v>11.000</v>
       </c>
       <c r="G228" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H228" s="3">
-        <v>2142.16</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7709,13 +7703,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>11.000</v>
+        <v>84.000</v>
       </c>
       <c r="G229" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H229" s="3">
-        <v>974.64</v>
+        <v>13440.76</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7735,13 +7729,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>84.000</v>
+        <v>168.620</v>
       </c>
       <c r="G230" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H230" s="3">
-        <v>13440.76</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7761,13 +7755,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>168.620</v>
+        <v>47.250</v>
       </c>
       <c r="G231" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H231" s="3">
-        <v>8798.84</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7787,13 +7781,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>47.250</v>
+        <v>22433.300</v>
       </c>
       <c r="G232" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H232" s="3">
-        <v>5148.59</v>
+        <v>50916.71</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7813,13 +7807,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>22433.300</v>
+        <v>2883.960</v>
       </c>
       <c r="G233" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H233" s="3">
-        <v>50916.71</v>
+        <v>12311.83</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7839,13 +7833,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>2883.960</v>
+        <v>29.390</v>
       </c>
       <c r="G234" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H234" s="3">
-        <v>12311.83</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7865,13 +7859,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>29.390</v>
+        <v>1198.180</v>
       </c>
       <c r="G235" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H235" s="3">
-        <v>15217.18</v>
+        <v>45050.39</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7891,13 +7885,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>1198.180</v>
+        <v>32.610</v>
       </c>
       <c r="G236" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H236" s="3">
-        <v>45050.39</v>
+        <v>333.10</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7917,13 +7911,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>32.610</v>
+        <v>35.000</v>
       </c>
       <c r="G237" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H237" s="3">
-        <v>333.10</v>
+        <v>783.60</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7943,13 +7937,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>35.000</v>
+        <v>1488.860</v>
       </c>
       <c r="G238" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H238" s="3">
-        <v>783.60</v>
+        <v>46774.71</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7969,13 +7963,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>1488.860</v>
+        <v>290.430</v>
       </c>
       <c r="G239" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H239" s="3">
-        <v>46774.71</v>
+        <v>26647.45</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7995,13 +7989,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>290.430</v>
+        <v>59.100</v>
       </c>
       <c r="G240" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H240" s="3">
-        <v>26647.45</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8021,13 +8015,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>59.100</v>
+        <v>241.900</v>
       </c>
       <c r="G241" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H241" s="3">
-        <v>9271.17</v>
+        <v>7817.79</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8047,13 +8041,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>241.900</v>
+        <v>154.000</v>
       </c>
       <c r="G242" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H242" s="3">
-        <v>7817.79</v>
+        <v>2851.98</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8073,13 +8067,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>154.000</v>
+        <v>0.690</v>
       </c>
       <c r="G243" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H243" s="3">
-        <v>2851.98</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8099,13 +8093,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>0.690</v>
+        <v>52.790</v>
       </c>
       <c r="G244" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H244" s="3">
-        <v>20.12</v>
+        <v>1134.03</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8125,13 +8119,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>52.790</v>
+        <v>78.310</v>
       </c>
       <c r="G245" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H245" s="3">
-        <v>1134.03</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8151,13 +8145,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>78.310</v>
+        <v>228.000</v>
       </c>
       <c r="G246" t="s">
-        <v>440</v>
+        <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>7083.14</v>
+        <v>1334.95</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8177,13 +8171,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>228.000</v>
+        <v>75.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>1334.95</v>
+        <v>413.17</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8203,13 +8197,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>75.000</v>
+        <v>4355.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>413.17</v>
+        <v>10932.56</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8229,13 +8223,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>4355.000</v>
+        <v>9.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>10932.56</v>
+        <v>3203.83</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8255,13 +8249,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>3203.83</v>
+        <v>556.74</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8281,13 +8275,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>1.000</v>
+        <v>11.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>556.74</v>
+        <v>4741.17</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8307,13 +8301,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>11.000</v>
+        <v>6.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>4741.17</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8333,13 +8327,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>2371.80</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8359,13 +8353,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>2323.99</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8385,13 +8379,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>6585.02</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8411,13 +8405,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>6.000</v>
+        <v>38.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>1694.29</v>
+        <v>17563.39</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8437,13 +8431,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>38.000</v>
+        <v>14.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>17563.39</v>
+        <v>7926.12</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8463,13 +8457,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>14.000</v>
+        <v>2.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>7926.12</v>
+        <v>3443.46</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8489,13 +8483,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>3443.46</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8515,13 +8509,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>6821.40</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8541,13 +8535,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>7220.40</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8567,13 +8561,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>7.000</v>
+        <v>18.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>2566.22</v>
+        <v>8283.69</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8593,13 +8587,13 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>18.000</v>
+        <v>7.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>8283.69</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -8619,13 +8613,13 @@
         <v>530</v>
       </c>
       <c r="F264" s="2">
-        <v>7.000</v>
+        <v>5.000</v>
       </c>
       <c r="G264" t="s">
         <v>5</v>
       </c>
       <c r="H264" s="3">
-        <v>3943.24</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="265" spans="1:8">
@@ -8645,38 +8639,12 @@
         <v>532</v>
       </c>
       <c r="F265" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G265" t="s">
         <v>5</v>
       </c>
       <c r="H265" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="266" spans="1:8">
-      <c r="A266" t="s">
-        <v>0</v>
-      </c>
-      <c r="B266" t="s">
-        <v>1</v>
-      </c>
-      <c r="C266" t="s">
-        <v>2</v>
-      </c>
-      <c r="D266" t="s">
-        <v>533</v>
-      </c>
-      <c r="E266" t="s">
-        <v>534</v>
-      </c>
-      <c r="F266" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H266" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>